<commit_message>
Stuff for the Tutorial  && Model Changes
- Creating the TextMeshs for the Tutorial steps
- Creating a Tutorial Manager Script and a Sript to set the Tutorial Step along
- Two New Tags: TubeB & TubeC

- New Materials for all Selfmade Objects
- Changeing the Firetruck so the pump have place inside
- Creating A Pylon
</commit_message>
<xml_diff>
--- a/RequiredModels/RequiredModels.xlsx
+++ b/RequiredModels/RequiredModels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Master\1.Semester\FortgeschritteneProgrammierung\Projekt\Project-Firefight\RequiredModels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2EBB944-418C-404D-8F16-3D1E0E6A9C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC66718D-5F3F-45E9-BCD9-410D240DA4F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -561,7 +561,7 @@
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,8 +955,8 @@
       <c r="C27" t="s">
         <v>45</v>
       </c>
-      <c r="D27" s="2">
-        <v>0</v>
+      <c r="D27" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
New Models and Changes at Old
New:
- A-Tube-Connection
- Saugkorb

Changed:
- Verteiler (Hebel seperated)
- Pumpe get 2 Hebel

Other Changes
- Balancing FireRulesVariable
- PylonClone Scrip
</commit_message>
<xml_diff>
--- a/RequiredModels/RequiredModels.xlsx
+++ b/RequiredModels/RequiredModels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Master\1.Semester\FortgeschritteneProgrammierung\Projekt\Project-Firefight\RequiredModels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC66718D-5F3F-45E9-BCD9-410D240DA4F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478240E6-A443-459E-A8A7-8D233E838F73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1590" yWindow="3195" windowWidth="23400" windowHeight="12555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -560,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>